<commit_message>
1) query for TQC 2) Construct for reification + query
</commit_message>
<xml_diff>
--- a/ChangeModels/change.xlsx
+++ b/ChangeModels/change.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trypuz/NetBeansProjects/ChangeModels/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trypuz/git_repo/change/ChangeModels/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>context</t>
   </si>
@@ -89,9 +89,6 @@
 } </t>
   </si>
   <si>
-    <t>SELECT ?s  WHERE {GRAPH &lt;http://onto.kul.pl/change/bfo-tqc&gt; { ?s a &lt;http://purl.obolibrary.org/obo/BFO_0000030&gt;} .}</t>
-  </si>
-  <si>
     <t>query 1</t>
   </si>
   <si>
@@ -138,9 +135,6 @@
   </si>
   <si>
     <t>http://lei.info/gleio</t>
-  </si>
-  <si>
-    <t>SELECT ?s  WHERE {GRAPH &lt;http://lei.info/gleio&gt; { ?s a &lt;http://lei.info/gleio/VariableEntity&gt;} .}</t>
   </si>
   <si>
     <t>gfo</t>
@@ -257,15 +251,6 @@
   </si>
   <si>
     <t>http://onto.kul.pl/change/namenesting</t>
-  </si>
-  <si>
-    <t>SELECT ?s  WHERE {GRAPH &lt;http://onto.kul.pl/change/gfo&gt; { ?s a ?c} .}</t>
-  </si>
-  <si>
-    <t>SELECT ?s  WHERE {GRAPH &lt;http://onto.kul.pl/change/temporalisedtriples&gt; { ?s a ?c} .}</t>
-  </si>
-  <si>
-    <t>SELECT ?s  WHERE {GRAPH &lt;http://onto.kul.pl/change/namenesting&gt; { ?s a ?c} .}</t>
   </si>
   <si>
     <t>PREFIX : &lt;http://lei.info/gleio/&gt;
@@ -321,6 +306,141 @@
   </si>
   <si>
     <t>http://onto.kul.pl/change/gfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PREFIX : &lt;http://lei.info/gleio/&gt;
+PREFIX reif: &lt;http://onto.kul.pl/change/reification/&gt;
+CONSTRUCT {
+?legalEntity a reif:LegalEntity ;
+        reif:hasReficationRelation ?manifestation.
+?manifestation a reif:RefificationRelation ;
+            reif:hasRefificationRelationCreationDate ?updateDate ;
+            reif:hasLegalEntityHeadquartersAddress ?headquartersAddress ;
+            reif:hasLegalEntityLegalName ?legalName.
+?headquartersAddress a :Address ;
+                     :hasCity ?city ;
+                     :hasCountry ?country ;
+                     :hasPostalCode ?postalCode ;
+                     :hasStreetAddress ?streetAddress ;
+                     :hasSubdivision ?subdivision .
+?country a :Country .
+?subdivision a :Subdivision . 
+reif:hasLegalEntityHeadquartersAddress a owl:ObjectProperty .  
+reif:hasReficationRelation a owl:ObjectProperty .  
+:hasCountry a owl:ObjectProperty .  
+:hasSubdivision a owl:ObjectProperty . 
+reif:hasRefificationRelationCreationDate a owl:DatatypeProperty .  
+reif:hasLegalEntityLegalName a owl:DatatypeProperty .
+:hasCity a owl:DatatypeProperty .
+:hasPostalCode a owl:DatatypeProperty .
+:hasStreetAddress a owl:DatatypeProperty .
+}
+WHERE {
+ ?legalEntity :hasManifestation ?manifestation .
+ ?manifestation :hasHeadquartersAddress ?headquartersAddress ;
+               :hasUpdateDate ?updateDate ;
+               :hasLegalName ?legalName.
+ ?headquartersAddress :hasCity ?city ;
+                     :hasCountry ?country ;
+                     :hasPostalCode ?postalCode ;
+                     :hasStreetAddress ?streetAddress ;
+                     :hasSubdivision ?subdivision .
+} </t>
+  </si>
+  <si>
+    <t>reification</t>
+  </si>
+  <si>
+    <t>http://onto.kul.pl/change/reification/</t>
+  </si>
+  <si>
+    <t>PREFIX :&lt;http://onto.kul.pl/change/gfo/&gt;
+SELECT ?legalName ?updateDate
+WHERE 
+{
+?legalEntitySlice :proper_part_of ?legalEntity .
+?legalEntitySlice :updateDate ?updateDate ;
+:hasLegalName ?legalName.
+FILTER (STR(?legalEntity)="http://lei.info/549300U5FI25Y6MFOS85#entity")
+FILTER (?updateDate &lt; "2016-09-23T10:20:13+05:30"^^xsd:dateTime)
+}
+ORDER BY DESC(?updateDate)
+LIMIT 1</t>
+  </si>
+  <si>
+    <t>PREFIX :&lt;http://onto.kul.pl/change/tripletemporalised/&gt;
+SELECT ?legalName ?updateDate
+WHERE 
+{
+?axiom rdf:type owl:Axiom ;
+owl:annotatedSource ?legalEntity ;
+owl:annotatedProperty :hasLegalName ;
+owl:annotatedTarget ?legalName ;
+:updateDate ?updateDate .
+FILTER (STR(?legalEntity)="http://lei.info/549300U5FI25Y6MFOS85#entity")
+FILTER (?updateDate &lt; "2016-09-23T10:20:13+05:30"^^xsd:dateTime)
+}
+ORDER BY DESC(?updateDate)
+LIMIT 1</t>
+  </si>
+  <si>
+    <t>PREFIX :&lt;http://onto.kul.pl/change/namenesting/&gt;
+SELECT ?legalName ?updateDate
+WHERE 
+{
+?legalEntityNameBlob :hasEntity ?legalEntity ;
+:updateDate ?updateDate ;
+:hasLegalName ?legalName.
+FILTER (STR(?legalEntity)="http://lei.info/549300U5FI25Y6MFOS85#entity")
+FILTER (?updateDate &lt; "2016-09-23T10:20:13+05:30"^^xsd:dateTime)
+}
+ORDER BY DESC(?updateDate)
+LIMIT 1</t>
+  </si>
+  <si>
+    <t>PREFIX : &lt;http://lei.info/gleio/&gt;
+SELECT ?legalName ?updateDate
+WHERE 
+{
+?legalEntity :hasManifestation ?manifestation .
+?manifestation :hasUpdateDate ?updateDate ;
+:hasLegalName ?legalName.
+FILTER (STR(?legalEntity)="http://lei.info/5493004R493UTY6GT060#entity")
+FILTER (?updateDate &lt; "2016-09-23T10:20:13+05:30"^^xsd:dateTime)
+}
+ORDER BY DESC(?updateDate)
+LIMIT 1</t>
+  </si>
+  <si>
+    <t>PREFIX : &lt;http://lei.info/gleio/&gt;
+PREFIX reif: &lt;http://onto.kul.pl/change/reification/&gt;
+SELECT ?legalName ?updateDate
+WHERE 
+{
+?legalEntity reif:hasReficationRelation ?manifestation .
+?manifestation reif:hasRefificationRelationCreationDate ?updateDate ;
+reif:hasLegalEntityLegalName ?legalName.
+FILTER (STR(?legalEntity)="http://lei.info/5493004R493UTY6GT060#entity")
+FILTER (?updateDate &lt; "2016-09-23T10:20:13+05:30"^^xsd:dateTime)
+}
+ORDER BY DESC(?updateDate)
+LIMIT 1</t>
+  </si>
+  <si>
+    <t>PREFIX : &lt;http://lei.info/gleio/&gt;
+SELECT ?legalName ?updateDate
+WHERE 
+{
+?legalEntity &lt;http://purl.obolibrary.org/obo/BFO_0000185&gt; ?legalEntityHistory .
+?legalEntityHistory &lt;http://purl.obolibrary.org/obo/BFO_0000117&gt; ?legalEntityPhase .
+?legalEntityPhase &lt;http://www.halbordnung.de/ontologies/tqc.owl#1669f0c5-4cde-5cbc-94e3-ffb2281d885a&gt; ?manifestation .
+?manifestation :hasUpdateDate ?updateDate ;
+  :hasLegalName ?legalName.
+FILTER (STR(?legalEntity)="http://lei.info/5493004R493UTY6GT060#entity")
+FILTER (?updateDate &lt; "2016-09-23T10:20:13+05:30"^^xsd:dateTime)
+}
+ORDER BY DESC(?updateDate)
+LIMIT 1</t>
   </si>
 </sst>
 </file>
@@ -742,15 +862,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="95.5" style="6" customWidth="1"/>
+    <col min="1" max="1" width="23" style="6" customWidth="1"/>
     <col min="2" max="2" width="86" customWidth="1"/>
     <col min="3" max="3" width="42.5" customWidth="1"/>
     <col min="4" max="4" width="63" customWidth="1"/>
@@ -767,49 +887,49 @@
         <v>0</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="256" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="409" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="204" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="9" t="s">
+      <c r="B4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="C4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>18</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="409" x14ac:dyDescent="0.2">
@@ -823,21 +943,35 @@
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="409" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>11</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="409" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>